<commit_message>
ITO-000 Create endpoint user-003
</commit_message>
<xml_diff>
--- a/document/user-endpoint.xlsx
+++ b/document/user-endpoint.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Context path</t>
   </si>
@@ -111,6 +111,48 @@
   </si>
   <si>
     <t>Get/Post</t>
+  </si>
+  <si>
+    <t>#user-003</t>
+  </si>
+  <si>
+    <t>Get user info by email</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>Description response</t>
+  </si>
+  <si>
+    <t>Message code</t>
+  </si>
+  <si>
+    <t>Message text</t>
+  </si>
+  <si>
+    <t>find success</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>onlinejudge.dto.MyResponse</t>
+  </si>
+  <si>
+    <t>email not exist</t>
+  </si>
+  <si>
+    <t>user.email.not.exist</t>
+  </si>
+  <si>
+    <t>Email [{0}] dose not exist.</t>
+  </si>
+  <si>
+    <t>Create success</t>
+  </si>
+  <si>
+    <t>Server error</t>
   </si>
 </sst>
 </file>
@@ -146,8 +188,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L7"/>
+  <dimension ref="A3:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,13 +553,15 @@
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="8" width="23.5703125" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="10" max="11" width="8.140625" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" customWidth="1"/>
+    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>0</v>
       </c>
@@ -522,7 +569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -554,13 +601,25 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
         <v>16</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -582,31 +641,94 @@
       <c r="J6" t="s">
         <v>10</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6">
+        <v>200</v>
+      </c>
+      <c r="L6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="N6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>500</v>
+      </c>
+      <c r="N7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I8" t="s">
         <v>27</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M8" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>200</v>
+      </c>
+      <c r="L9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>400</v>
+      </c>
+      <c r="L10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ITO-000 update API create User
</commit_message>
<xml_diff>
--- a/document/user-endpoint.xlsx
+++ b/document/user-endpoint.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Context path</t>
   </si>
@@ -153,6 +153,22 @@
   </si>
   <si>
     <t>Server error</t>
+  </si>
+  <si>
+    <t>{
+  "email":"hoangnhuocquy@csc.com",
+  "password":"P@ssword123",
+  "displayName":"Hoang Nhuoc QUy"
+}</t>
+  </si>
+  <si>
+    <t>User exist</t>
+  </si>
+  <si>
+    <t>user.create.exist</t>
+  </si>
+  <si>
+    <t>User exist with email [{0}]</t>
   </si>
 </sst>
 </file>
@@ -188,10 +204,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,10 +557,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:P10"/>
+  <dimension ref="A3:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +638,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -638,6 +657,9 @@
       <c r="G6" t="s">
         <v>15</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J6" t="s">
         <v>10</v>
       </c>
@@ -645,55 +667,50 @@
         <v>200</v>
       </c>
       <c r="L6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="N6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
       <c r="K7">
+        <v>400</v>
+      </c>
+      <c r="L7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K8">
         <v>500</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N8" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
         <v>27</v>
@@ -701,33 +718,56 @@
       <c r="I9" t="s">
         <v>27</v>
       </c>
-      <c r="J9" t="s">
+      <c r="M9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
         <v>10</v>
       </c>
-      <c r="K9">
+      <c r="K10">
         <v>200</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L10" t="s">
         <v>15</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K10">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K11">
         <v>400</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L11" t="s">
         <v>40</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N11" t="s">
         <v>41</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O11" t="s">
         <v>42</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P11" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>